<commit_message>
Add test cases and tasks to project.xlsx.
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="125">
   <si>
     <t>TC Number</t>
   </si>
@@ -370,6 +370,42 @@
   </si>
   <si>
     <t>JS Linter</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Create new account then log in / log out</t>
+  </si>
+  <si>
+    <t>Create new poem with pre-existing account</t>
+  </si>
+  <si>
+    <t>Navigate to user management page with pre-exisitng admin account</t>
+  </si>
+  <si>
+    <t>While not logged in, view details of one poem then navigate to the homepage</t>
+  </si>
+  <si>
+    <t>Feature not  implemented</t>
+  </si>
+  <si>
+    <t>Basic log in / log out with pre-existing non-admin account</t>
+  </si>
+  <si>
+    <t>Basic log in / log out with pre-existing admin account.  View user admin page.</t>
+  </si>
+  <si>
+    <t>In progress with Selenium</t>
+  </si>
+  <si>
+    <t>Poem details page should have buttons to share on social media</t>
+  </si>
+  <si>
+    <t>Create 1000 local user accounts</t>
+  </si>
+  <si>
+    <t>IP</t>
   </si>
 </sst>
 </file>
@@ -438,7 +474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -449,6 +485,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -768,7 +805,7 @@
   <dimension ref="A1:D704"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1148,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>132</v>
       </c>
@@ -1119,7 +1156,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>133</v>
       </c>
@@ -1127,7 +1164,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>134</v>
       </c>
@@ -1135,7 +1172,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>135</v>
       </c>
@@ -1143,7 +1180,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>136</v>
       </c>
@@ -1151,7 +1188,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>137</v>
       </c>
@@ -1159,7 +1196,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>138</v>
       </c>
@@ -1167,7 +1204,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>139</v>
       </c>
@@ -1175,45 +1212,54 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>140</v>
       </c>
+      <c r="B41" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="C41" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>141</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>147</v>
       </c>
@@ -4514,8 +4560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4883,6 +4929,9 @@
       <c r="C29" t="s">
         <v>52</v>
       </c>
+      <c r="D29" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -4923,82 +4972,133 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>131</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>132</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>133</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>134</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>135</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>136</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>137</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>142</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
Changes to unit tests.
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="143">
   <si>
     <t>TC Number</t>
   </si>
@@ -318,18 +318,12 @@
     <t>Admin interface for all poems</t>
   </si>
   <si>
-    <t>Admin interface for users needs paging and sorting</t>
-  </si>
-  <si>
     <t>In the DB, each line should be associated with the UUID of the user who wrote it.  Will require new schema!</t>
   </si>
   <si>
     <t>User interface for viewing and managing own poems.  "My poems"</t>
   </si>
   <si>
-    <t>When a poem is created, a user should be sent to the "My poems" page.</t>
-  </si>
-  <si>
     <t>Find a way to allow users to simply type a sentence and submit rather than filling in x number of text boxes.  Idea from Filip.</t>
   </si>
   <si>
@@ -447,7 +441,25 @@
     <t>Hide all but title, tail, and previous line being edited when editing</t>
   </si>
   <si>
-    <t>Until a poem is complete, only the title and tail should be visibile on the homepage</t>
+    <t>When a poem is created, a user should be sent to their "My poems" page.</t>
+  </si>
+  <si>
+    <t>Poem entry should have words on one line rather than stacked on top of each other</t>
+  </si>
+  <si>
+    <t>Until a poem is complete, only the title and tail should be visibile on the homepage and in edit view</t>
+  </si>
+  <si>
+    <t>Implement free-form text search of entire database of poems</t>
+  </si>
+  <si>
+    <t>Admin interface for users needs sorting</t>
+  </si>
+  <si>
+    <t>Duplicate of 142</t>
+  </si>
+  <si>
+    <t>dup</t>
   </si>
 </sst>
 </file>
@@ -868,7 +880,7 @@
   <dimension ref="A1:D704"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1044,7 @@
         <v>74</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1043,7 +1055,7 @@
         <v>75</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1054,10 +1066,10 @@
         <v>38</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1090,7 +1102,7 @@
         <v>117</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1128,7 +1140,7 @@
         <v>121</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1136,7 +1148,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1150,7 +1162,7 @@
         <v>83</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1196,7 +1208,7 @@
         <v>128</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,12 +1270,18 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>136</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>95</v>
+      <c r="B37" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1271,15 +1289,15 @@
         <v>137</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>138</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>98</v>
+      <c r="C39" s="5" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1287,7 +1305,7 @@
         <v>139</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1298,10 +1316,10 @@
         <v>38</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1309,23 +1327,30 @@
         <v>141</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>142</v>
       </c>
+      <c r="B43" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="C43" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>143</v>
       </c>
+      <c r="B44" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="C44" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1336,19 +1361,31 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>145</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>146</v>
       </c>
+      <c r="C47" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>147</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
@@ -4838,7 +4875,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -4915,10 +4952,10 @@
         <v>46</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4929,10 +4966,10 @@
         <v>46</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -4943,10 +4980,10 @@
         <v>46</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -4960,7 +4997,7 @@
         <v>47</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -5018,7 +5055,7 @@
         <v>51</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -5040,10 +5077,10 @@
         <v>46</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -5054,10 +5091,10 @@
         <v>46</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5065,13 +5102,13 @@
         <v>131</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -5079,13 +5116,13 @@
         <v>132</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5093,13 +5130,13 @@
         <v>133</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -5107,13 +5144,13 @@
         <v>134</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -5121,13 +5158,13 @@
         <v>135</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -5135,13 +5172,13 @@
         <v>136</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -5149,13 +5186,13 @@
         <v>137</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>129</v>
-      </c>
       <c r="D39" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -5163,13 +5200,13 @@
         <v>138</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>